<commit_message>
Entrance added to report
</commit_message>
<xml_diff>
--- a/Web/templates/report.xlsx
+++ b/Web/templates/report.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F379576-3C0D-44D2-809B-37A98E0B66E1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710C356E-9F49-4A01-BD58-BEA58E0D3C5D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>День</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>Строгий график</t>
+  </si>
+  <si>
+    <t>Место</t>
   </si>
 </sst>
 </file>
@@ -102,13 +105,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -389,50 +392,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
     <col min="2" max="2" width="40.7109375" customWidth="1"/>
-    <col min="3" max="7" width="20.7109375" customWidth="1"/>
+    <col min="3" max="8" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C5" s="4" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -446,12 +449,15 @@
         <v>3</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>